<commit_message>
Amlak private New Columns-  excel import
</commit_message>
<xml_diff>
--- a/NewsWebsite/wwwroot/excel_templetes/amlak_private.xlsx
+++ b/NewsWebsite/wwwroot/excel_templetes/amlak_private.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\ASP\Erp_Project\NewsWebsite\wwwroot\excel_templetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6058DBAE-CA1A-4048-A734-2BFA66A808AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45B04A6-3D9D-4A71-80CE-9FEFFB2BD3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7F283721-637C-4500-B8C0-83D034281840}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7F283721-637C-4500-B8C0-83D034281840}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,9 +61,6 @@
     <t>کد سادا</t>
   </si>
   <si>
-    <t>کد سجام</t>
-  </si>
-  <si>
     <t>کد SDI</t>
   </si>
   <si>
@@ -77,6 +74,9 @@
   </si>
   <si>
     <t>پیشبینی استفاده</t>
+  </si>
+  <si>
+    <t>کد جام</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,22 +490,22 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>